<commit_message>
minor change in testcase_7
</commit_message>
<xml_diff>
--- a/src/main/java/resources/testData/TestData.xlsx
+++ b/src/main/java/resources/testData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsingh\.jenkins\${JENKIN_HOME}\ECP_VW\src\main\java\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsingh\git_project\ECP_VW\src\main\java\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -180,7 +180,7 @@
     <t>PARTCLINET_USER</t>
   </si>
   <si>
-    <t>Partner/User1</t>
+    <t>Partner/User</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Bug fix of test tab
</commit_message>
<xml_diff>
--- a/src/main/java/resources/testData/TestData.xlsx
+++ b/src/main/java/resources/testData/TestData.xlsx
@@ -512,13 +512,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>